<commit_message>
asserts sur les valeurs extraites du fichier eurostar dessertes & refactoring de l'étape d'extraction des tables de ref
</commit_message>
<xml_diff>
--- a/src/test/resources/testFiles/rapportDeControle/EurostarDessertesTest1.xlsx
+++ b/src/test/resources/testFiles/rapportDeControle/EurostarDessertesTest1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="71">
   <si>
     <t>Eurostar Timetable - Period D2 2016: London to Paris</t>
   </si>
@@ -424,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -548,6 +548,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -967,7 +970,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,8 +1082,8 @@
       <c r="F9" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>17</v>
+      <c r="G9" s="48">
+        <v>0.34166999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1954,12 +1957,13 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE64"/>
+  <dimension ref="A1:Y64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>

</xml_diff>

<commit_message>
import dessertes double meal : test & bug fix
</commit_message>
<xml_diff>
--- a/src/test/resources/testFiles/rapportDeControle/EurostarDessertesTest1.xlsx
+++ b/src/test/resources/testFiles/rapportDeControle/EurostarDessertesTest1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="71">
   <si>
     <t>Eurostar Timetable - Period D2 2016: London to Paris</t>
   </si>
@@ -424,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -550,6 +550,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -967,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,67 +1847,85 @@
     </row>
     <row r="61" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F61" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G61" s="49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C61" s="46">
-        <f t="shared" ref="C61:G61" si="0">C$16-C$7-TIME(1,0,0)</f>
+      <c r="C62" s="46">
+        <f t="shared" ref="C62:G62" si="0">C$16-C$7-TIME(1,0,0)</f>
         <v>0.10902777777777778</v>
       </c>
-      <c r="D61" s="46">
+      <c r="D62" s="46">
         <f t="shared" si="0"/>
         <v>0.10347222222222222</v>
       </c>
-      <c r="E61" s="46">
+      <c r="E62" s="46">
         <f t="shared" si="0"/>
         <v>9.4444444444444414E-2</v>
       </c>
-      <c r="F61" s="46">
+      <c r="F62" s="46">
         <f t="shared" si="0"/>
         <v>0.10069444444444445</v>
       </c>
-      <c r="G61" s="46">
+      <c r="G62" s="46">
         <f t="shared" si="0"/>
         <v>9.8611111111111122E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="34" t="s">
+    <row r="63" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="C62" s="36" t="s">
+      <c r="C63" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="D62" s="36" t="s">
+      <c r="D63" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="E62" s="36" t="s">
+      <c r="E63" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="F62" s="36" t="s">
+      <c r="F63" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="G62" s="36" t="s">
+      <c r="G63" s="36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="3">
+    <row r="64" spans="2:7" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="3">
         <v>1</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D64" s="3">
         <v>2</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E64" s="3">
         <v>3</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F64" s="3">
         <v>4</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G64" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="C17:G23">
     <cfRule type="containsBlanks" dxfId="15" priority="10">

</xml_diff>